<commit_message>
hcamacho: se ve leecion 3
</commit_message>
<xml_diff>
--- a/AvancesCurso.xlsx
+++ b/AvancesCurso.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcamacho\Documents\C# PildorasInformaticas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcamacho\Documents\C-PildorasInformaticas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E458A61-2650-4A6E-B239-818061D02C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B919C7-D960-4920-863D-4A5C5F61B2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6585" windowWidth="29040" windowHeight="15840" xr2:uid="{A6EFA792-59B4-45BA-A396-5FAB1D5E35B1}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7360" xr2:uid="{A6EFA792-59B4-45BA-A396-5FAB1D5E35B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -179,6 +179,8 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,13 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="9" tint="-0.24994659260841701"/>
@@ -212,11 +212,6 @@
     <dxf>
       <font>
         <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
   </dxfs>
@@ -529,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F4D655-B3BF-49E9-A8AB-EB8D810259EA}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -545,1042 +540,1042 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="7">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="7">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="7">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="7">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="7">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="7">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="7">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="7">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="7">
-        <v>0</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="7">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="7">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="7">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="7">
-        <v>0</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="7">
-        <v>0</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="7">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="7">
-        <v>0</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="7">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="7">
-        <v>0</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="7">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="7">
-        <v>0</v>
-      </c>
-      <c r="C28" s="7">
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="7">
-        <v>0</v>
-      </c>
-      <c r="C29" s="7">
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
         <v>23</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="7">
-        <v>0</v>
-      </c>
-      <c r="C30" s="7">
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="7">
-        <v>0</v>
-      </c>
-      <c r="C31" s="7">
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="7">
-        <v>0</v>
-      </c>
-      <c r="C32" s="7">
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="7">
-        <v>0</v>
-      </c>
-      <c r="C33" s="7">
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
         <v>27</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="7">
-        <v>0</v>
-      </c>
-      <c r="C34" s="7">
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="7">
-        <v>0</v>
-      </c>
-      <c r="C35" s="7">
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="7">
-        <v>0</v>
-      </c>
-      <c r="C36" s="7">
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
         <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="7">
-        <v>0</v>
-      </c>
-      <c r="C37" s="7">
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="7">
-        <v>0</v>
-      </c>
-      <c r="C38" s="7">
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="7">
-        <v>0</v>
-      </c>
-      <c r="C39" s="7">
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
         <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="7">
-        <v>0</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="7">
-        <v>0</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="7">
-        <v>0</v>
-      </c>
-      <c r="C42" s="7">
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
         <v>36</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="7">
-        <v>0</v>
-      </c>
-      <c r="C43" s="7">
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
         <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="7">
-        <v>0</v>
-      </c>
-      <c r="C44" s="7">
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="7">
-        <v>0</v>
-      </c>
-      <c r="C45" s="7">
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
         <v>39</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="7">
-        <v>0</v>
-      </c>
-      <c r="C46" s="7">
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="7">
-        <v>0</v>
-      </c>
-      <c r="C47" s="7">
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="7">
-        <v>0</v>
-      </c>
-      <c r="C48" s="7">
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
         <v>42</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="7">
-        <v>0</v>
-      </c>
-      <c r="C49" s="7">
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="7">
-        <v>0</v>
-      </c>
-      <c r="C50" s="7">
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
         <v>44</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="7">
-        <v>0</v>
-      </c>
-      <c r="C51" s="7">
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
         <v>45</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="7">
-        <v>0</v>
-      </c>
-      <c r="C52" s="7">
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1">
         <v>46</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="7">
-        <v>0</v>
-      </c>
-      <c r="C53" s="7">
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
         <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="7">
-        <v>0</v>
-      </c>
-      <c r="C54" s="7">
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="7">
-        <v>0</v>
-      </c>
-      <c r="C55" s="7">
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
         <v>49</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="7">
-        <v>0</v>
-      </c>
-      <c r="C56" s="7">
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="7">
-        <v>0</v>
-      </c>
-      <c r="C57" s="7">
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="7">
-        <v>0</v>
-      </c>
-      <c r="C58" s="7">
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
         <v>52</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="7">
-        <v>0</v>
-      </c>
-      <c r="C59" s="7">
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
         <v>53</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="7">
-        <v>0</v>
-      </c>
-      <c r="C60" s="7">
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
         <v>54</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="7">
-        <v>0</v>
-      </c>
-      <c r="C61" s="7">
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
         <v>55</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="7">
-        <v>0</v>
-      </c>
-      <c r="C62" s="7">
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
         <v>56</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="7">
-        <v>0</v>
-      </c>
-      <c r="C63" s="7">
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
         <v>57</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="7">
-        <v>0</v>
-      </c>
-      <c r="C64" s="7">
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
         <v>58</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="7">
-        <v>0</v>
-      </c>
-      <c r="C65" s="7">
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66" s="7">
-        <v>0</v>
-      </c>
-      <c r="C66" s="7">
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67" s="7">
-        <v>0</v>
-      </c>
-      <c r="C67" s="7">
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
         <v>61</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="7">
-        <v>0</v>
-      </c>
-      <c r="C68" s="7">
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
         <v>62</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="7">
-        <v>0</v>
-      </c>
-      <c r="C69" s="7">
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
         <v>63</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="7">
-        <v>0</v>
-      </c>
-      <c r="C70" s="7">
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
         <v>64</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="7">
-        <v>0</v>
-      </c>
-      <c r="C71" s="7">
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
         <v>65</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="7">
-        <v>0</v>
-      </c>
-      <c r="C72" s="7">
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
         <v>66</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="7">
-        <v>0</v>
-      </c>
-      <c r="C73" s="7">
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
         <v>67</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="7">
-        <v>0</v>
-      </c>
-      <c r="C74" s="7">
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
         <v>68</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="7">
-        <v>0</v>
-      </c>
-      <c r="C75" s="7">
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76" s="7">
-        <v>0</v>
-      </c>
-      <c r="C76" s="7">
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="7">
-        <v>0</v>
-      </c>
-      <c r="C77" s="7">
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
         <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="7">
-        <v>0</v>
-      </c>
-      <c r="C78" s="7">
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
         <v>72</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="7">
-        <v>0</v>
-      </c>
-      <c r="C79" s="7">
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
         <v>73</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="7">
-        <v>0</v>
-      </c>
-      <c r="C80" s="7">
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
         <v>74</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="7">
-        <v>0</v>
-      </c>
-      <c r="C81" s="7">
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82" s="7">
-        <v>0</v>
-      </c>
-      <c r="C82" s="7">
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
         <v>76</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="7">
-        <v>0</v>
-      </c>
-      <c r="C83" s="7">
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
         <v>77</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84" s="7">
-        <v>0</v>
-      </c>
-      <c r="C84" s="7">
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1">
         <v>78</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85" s="7">
-        <v>0</v>
-      </c>
-      <c r="C85" s="7">
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1">
         <v>79</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="7">
-        <v>0</v>
-      </c>
-      <c r="C86" s="7">
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
         <v>80</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="7">
-        <v>0</v>
-      </c>
-      <c r="C87" s="7">
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
         <v>81</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88" s="7">
-        <v>0</v>
-      </c>
-      <c r="C88" s="7">
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1">
         <v>82</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="7">
-        <v>0</v>
-      </c>
-      <c r="C89" s="7">
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="C89" s="1">
         <v>83</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90" s="7">
-        <v>0</v>
-      </c>
-      <c r="C90" s="7">
+      <c r="B90" s="1">
+        <v>0</v>
+      </c>
+      <c r="C90" s="1">
         <v>84</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91" s="7">
-        <v>0</v>
-      </c>
-      <c r="C91" s="7">
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1">
         <v>85</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92" s="7">
-        <v>0</v>
-      </c>
-      <c r="C92" s="7">
+      <c r="B92" s="1">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1">
         <v>86</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93" s="7">
-        <v>0</v>
-      </c>
-      <c r="C93" s="7">
+      <c r="B93" s="1">
+        <v>0</v>
+      </c>
+      <c r="C93" s="1">
         <v>87</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="7">
-        <v>0</v>
-      </c>
-      <c r="C94" s="7">
+      <c r="B94" s="1">
+        <v>0</v>
+      </c>
+      <c r="C94" s="1">
         <v>88</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="7">
-        <v>0</v>
-      </c>
-      <c r="C95" s="7">
+      <c r="B95" s="1">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1">
         <v>89</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="7">
-        <v>0</v>
-      </c>
-      <c r="C96" s="7">
+      <c r="B96" s="1">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1">
         <v>90</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="7">
-        <v>0</v>
-      </c>
-      <c r="C97" s="7">
+      <c r="B97" s="1">
+        <v>0</v>
+      </c>
+      <c r="C97" s="1">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98" s="7">
-        <v>0</v>
-      </c>
-      <c r="C98" s="7">
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1">
         <v>92</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99" s="7">
-        <v>0</v>
-      </c>
-      <c r="C99" s="7">
+      <c r="B99" s="1">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1">
         <v>93</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100" s="7">
-        <v>0</v>
-      </c>
-      <c r="C100" s="7">
+      <c r="B100" s="1">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1">
         <v>94</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B101" s="7">
-        <v>0</v>
-      </c>
-      <c r="C101" s="7">
+      <c r="B101" s="1">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1">
         <v>95</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="7">
-        <v>0</v>
-      </c>
-      <c r="C102" s="7">
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1">
         <v>96</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B103" s="7">
-        <v>0</v>
-      </c>
-      <c r="C103" s="7">
+      <c r="B103" s="1">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1">
         <v>97</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B104" s="7">
-        <v>0</v>
-      </c>
-      <c r="C104" s="7">
+      <c r="B104" s="1">
+        <v>0</v>
+      </c>
+      <c r="C104" s="1">
         <v>98</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B105" s="7">
-        <v>0</v>
-      </c>
-      <c r="C105" s="7">
+      <c r="B105" s="1">
+        <v>0</v>
+      </c>
+      <c r="C105" s="1">
         <v>99</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="7">
-        <v>0</v>
-      </c>
-      <c r="C106" s="7">
+      <c r="B106" s="1">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="7">
-        <v>0</v>
-      </c>
-      <c r="C107" s="7">
+      <c r="B107" s="1">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1">
         <v>101</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B108" s="7">
-        <v>0</v>
-      </c>
-      <c r="C108" s="7">
+      <c r="B108" s="1">
+        <v>0</v>
+      </c>
+      <c r="C108" s="1">
         <v>102</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B109" s="7">
-        <v>0</v>
-      </c>
-      <c r="C109" s="7">
+      <c r="B109" s="1">
+        <v>0</v>
+      </c>
+      <c r="C109" s="1">
         <v>103</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B110" s="7">
-        <v>0</v>
-      </c>
-      <c r="C110" s="7">
+      <c r="B110" s="1">
+        <v>0</v>
+      </c>
+      <c r="C110" s="1">
         <v>104</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B111" s="7">
-        <v>0</v>
-      </c>
-      <c r="C111" s="7">
+      <c r="B111" s="1">
+        <v>0</v>
+      </c>
+      <c r="C111" s="1">
         <v>105</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B112" s="7">
-        <v>0</v>
-      </c>
-      <c r="C112" s="7">
+      <c r="B112" s="1">
+        <v>0</v>
+      </c>
+      <c r="C112" s="1">
         <v>106</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B113" s="7">
-        <v>0</v>
-      </c>
-      <c r="C113" s="7">
+      <c r="B113" s="1">
+        <v>0</v>
+      </c>
+      <c r="C113" s="1">
         <v>107</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B114" s="7">
-        <v>0</v>
-      </c>
-      <c r="C114" s="7">
+      <c r="B114" s="1">
+        <v>0</v>
+      </c>
+      <c r="C114" s="1">
         <v>108</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B115" s="7">
-        <v>0</v>
-      </c>
-      <c r="C115" s="7">
+      <c r="B115" s="1">
+        <v>0</v>
+      </c>
+      <c r="C115" s="1">
         <v>109</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B116" s="7">
-        <v>0</v>
-      </c>
-      <c r="C116" s="7">
+      <c r="B116" s="1">
+        <v>0</v>
+      </c>
+      <c r="C116" s="1">
         <v>110</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B117" s="7">
-        <v>0</v>
-      </c>
-      <c r="C117" s="7">
+      <c r="B117" s="1">
+        <v>0</v>
+      </c>
+      <c r="C117" s="1">
         <v>111</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B118" s="7">
-        <v>0</v>
-      </c>
-      <c r="C118" s="7">
+      <c r="B118" s="1">
+        <v>0</v>
+      </c>
+      <c r="C118" s="1">
         <v>112</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B119" s="7">
-        <v>0</v>
-      </c>
-      <c r="C119" s="7">
+      <c r="B119" s="1">
+        <v>0</v>
+      </c>
+      <c r="C119" s="1">
         <v>113</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B120" s="7">
-        <v>0</v>
-      </c>
-      <c r="C120" s="7">
+      <c r="B120" s="1">
+        <v>0</v>
+      </c>
+      <c r="C120" s="1">
         <v>114</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B121" s="7">
-        <v>0</v>
-      </c>
-      <c r="C121" s="7">
+      <c r="B121" s="1">
+        <v>0</v>
+      </c>
+      <c r="C121" s="1">
         <v>115</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B122" s="7">
-        <v>0</v>
-      </c>
-      <c r="C122" s="7">
+      <c r="B122" s="1">
+        <v>0</v>
+      </c>
+      <c r="C122" s="1">
         <v>116</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B123" s="7">
-        <v>0</v>
-      </c>
-      <c r="C123" s="7">
+      <c r="B123" s="1">
+        <v>0</v>
+      </c>
+      <c r="C123" s="1">
         <v>117</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B124" s="7">
-        <v>0</v>
-      </c>
-      <c r="C124" s="7">
+      <c r="B124" s="1">
+        <v>0</v>
+      </c>
+      <c r="C124" s="1">
         <v>118</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B125" s="7">
-        <v>0</v>
-      </c>
-      <c r="C125" s="7">
+      <c r="B125" s="1">
+        <v>0</v>
+      </c>
+      <c r="C125" s="1">
         <v>119</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B126" s="7">
-        <v>0</v>
-      </c>
-      <c r="C126" s="7">
+      <c r="B126" s="1">
+        <v>0</v>
+      </c>
+      <c r="C126" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B127" s="7">
-        <v>0</v>
-      </c>
-      <c r="C127" s="7">
+      <c r="B127" s="1">
+        <v>0</v>
+      </c>
+      <c r="C127" s="1">
         <v>121</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B128" s="7">
-        <v>0</v>
-      </c>
-      <c r="C128" s="7">
+      <c r="B128" s="1">
+        <v>0</v>
+      </c>
+      <c r="C128" s="1">
         <v>122</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B129" s="7">
-        <v>0</v>
-      </c>
-      <c r="C129" s="7">
+      <c r="B129" s="1">
+        <v>0</v>
+      </c>
+      <c r="C129" s="1">
         <v>123</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B130" s="7">
-        <v>0</v>
-      </c>
-      <c r="C130" s="7">
+      <c r="B130" s="1">
+        <v>0</v>
+      </c>
+      <c r="C130" s="1">
         <v>124</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B131" s="7">
-        <v>0</v>
-      </c>
-      <c r="C131" s="7">
+      <c r="B131" s="1">
+        <v>0</v>
+      </c>
+      <c r="C131" s="1">
         <v>125</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B132" s="7">
-        <v>0</v>
-      </c>
-      <c r="C132" s="7">
+      <c r="B132" s="1">
+        <v>0</v>
+      </c>
+      <c r="C132" s="1">
         <v>126</v>
       </c>
     </row>
@@ -1590,6 +1585,12 @@
     <mergeCell ref="B2:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B132">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1598,12 +1599,6 @@
         <color theme="9" tint="-0.249977111117893"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
hcamacho: se avanza hasta la clase 6
</commit_message>
<xml_diff>
--- a/AvancesCurso.xlsx
+++ b/AvancesCurso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcamacho\Documents\C-PildorasInformaticas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B919C7-D960-4920-863D-4A5C5F61B2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9286B136-EB84-42D8-951B-54FCEA4306BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7360" xr2:uid="{A6EFA792-59B4-45BA-A396-5FAB1D5E35B1}"/>
+    <workbookView xWindow="-28920" yWindow="-6585" windowWidth="29040" windowHeight="15840" xr2:uid="{A6EFA792-59B4-45BA-A396-5FAB1D5E35B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>5</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>

</xml_diff>

<commit_message>
hcamacho: se ve hasta la clase 8
</commit_message>
<xml_diff>
--- a/AvancesCurso.xlsx
+++ b/AvancesCurso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcamacho\Documents\C-PildorasInformaticas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9286B136-EB84-42D8-951B-54FCEA4306BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEA2CD0-7410-4865-9481-1BF987925719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-6585" windowWidth="29040" windowHeight="15840" xr2:uid="{A6EFA792-59B4-45BA-A396-5FAB1D5E35B1}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>7</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
         <v>8</v>

</xml_diff>